<commit_message>
finish ETL and analysis; reorganize; finish readme
</commit_message>
<xml_diff>
--- a/data_dictionary.xlsx
+++ b/data_dictionary.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="64">
   <si>
     <t xml:space="preserve">table</t>
   </si>
@@ -28,13 +28,190 @@
     <t xml:space="preserve">column</t>
   </si>
   <si>
-    <t xml:space="preserve">datatype</t>
-  </si>
-  <si>
     <t xml:space="preserve">description</t>
   </si>
   <si>
-    <t xml:space="preserve">source</t>
+    <t xml:space="preserve">solar_metrics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">primary key ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zip_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US 5-digit zip code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">percent_qualified_bldgs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percent of buildings in area qualified for solar installs in a zip code.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number_potential_panels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of potential solar panels that could be installed on residential buildings in a zip code.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kw_median</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Median kW of power on a residential roof in a zip code.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">potential_installs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number ofresidential buildings for potential residential solar installs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">median_income</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Median income of the zip code.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">median_age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Median age of the zip code area.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">occupied_housing_units</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of housing units in the zip code that are occupied.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">owner_occupied_housing_units</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of housing units in the zip code occupied by owners.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">family_homes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of single-family homes (attached/detached) and residential buildings sized up to 4-family buildings.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">collegiates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of people with at least a bachelors degree.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moved_recently</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of people who moved within the last year.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">average_yearly_electric_bill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The average electric bill in dollars for the zip code area.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">average_yearly_kwh_used</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average number of kWh used in the zip code area.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">installer_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID for the primary installer for the zip code area.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">battery_system_fraction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fraction of houses with a solar install from the LBNL survey that have a battery system installed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mean_annual_feedin_tariff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The average feedin tariff payment for the area from the LBNL survey (from homes with an installed solar system).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zipcodes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zipcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The US 5-digit zip code.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">city_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name of the US city associated with the zip code.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">state_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name of the US state containing the zip code.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">latitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Latitude of the zip code (assuming it’s the central of mass of the zipcode).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Longitude of the zip code (assuming it’s the central of mass of the zipcode).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">utility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">utility_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name of the primary utility company that serves the zip code.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ownership</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The type of ownership (e.g. instritutional, state, coop) of the utility company.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">service_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type of service (e.g. Bundled, Delivery) of the utility.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">installer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unique ID for the installer.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">installer_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name of the installer.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">installer_primary_module_manufacturer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The most-used module manufacturer for that installer.</t>
   </si>
 </sst>
 </file>
@@ -49,6 +226,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -130,10 +308,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -151,11 +329,335 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="0" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>4</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>